<commit_message>
Add more tests and update tests.xlsx
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\176617\se-lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52568CB-B0BC-4CAC-83A2-D55ADC0816F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41D6C11-C9E1-41F0-9178-AA7D01DC61EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="5" xr2:uid="{A8991115-B65E-4ADC-B90F-2237A90A6CC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8991115-B65E-4ADC-B90F-2237A90A6CC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Teszteset #1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,12 @@
     <sheet name="Teszteset #4" sheetId="4" r:id="rId4"/>
     <sheet name="Teszteset #5" sheetId="5" r:id="rId5"/>
     <sheet name="Teszteset #6" sheetId="7" r:id="rId6"/>
+    <sheet name="Teszteset #7" sheetId="8" r:id="rId7"/>
+    <sheet name="Teszteset #8" sheetId="9" r:id="rId8"/>
+    <sheet name="Teszteset #9" sheetId="10" r:id="rId9"/>
+    <sheet name="Teszteset #10" sheetId="11" r:id="rId10"/>
+    <sheet name="Teszteset #11" sheetId="12" r:id="rId11"/>
+    <sheet name="Teszteset #12" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t>Tesztelt követelmény</t>
   </si>
@@ -111,6 +117,54 @@
   </si>
   <si>
     <t>Tüzelünk mindkét torpedóval, pl.: TORPEDO,ALL</t>
+  </si>
+  <si>
+    <t>A GT4500 elsődleges fegyvere újra lő, ha a másodlagos üres</t>
+  </si>
+  <si>
+    <t>Az elsődleges fegyverben 2 torpedó van (és a failure rate 0) és a másodlagosban 0</t>
+  </si>
+  <si>
+    <t>A GT4500 mindkét fegyvere üres, ezért nem tud tüzelni</t>
+  </si>
+  <si>
+    <t>Mindkét fegyverben pontosan 0 torpedó van</t>
+  </si>
+  <si>
+    <t>Mindkét tüzelés eredménye FAIL</t>
+  </si>
+  <si>
+    <t>A GT4500 elsődleges fegyverében 1 torpedó, de kétszer próbálunk meg tüzelni</t>
+  </si>
+  <si>
+    <t>Az elsődleges fegyverben pontosan 1 torpedó, míg a másodikban pontosan 0 torpedo</t>
+  </si>
+  <si>
+    <t>Az első eredménye SUCCESS, a másodiké FAIL</t>
+  </si>
+  <si>
+    <t>A GT4500 mindkét fegyvere üres, de mindet megpróbáljuk tüzelni</t>
+  </si>
+  <si>
+    <t>Pontosan 0 torpedó található mindkét fegyverben</t>
+  </si>
+  <si>
+    <t>A tüzelés eredménye FAIL</t>
+  </si>
+  <si>
+    <t>Tüzeljük mindkét torpedót, pl.: TORPEDO,ALL</t>
+  </si>
+  <si>
+    <t>Az elsődleges fegyverben 1, a másodlagos fegyverben 0 torpedó</t>
+  </si>
+  <si>
+    <t>A GT4500 elsődleges fegyverében 0, másodlagos fegyverében 1 torpedó és mindet megpróbáljuk tüzelni</t>
+  </si>
+  <si>
+    <t>Az elsődleges fegyverben 0, a másodlagos fegyverben 1 torpedó</t>
+  </si>
+  <si>
+    <t>A GT4500 elsődleges fegyverében 1, másodlagos fegyverében 0 torpedó és mindet megpróbáljuk tüzelni</t>
   </si>
 </sst>
 </file>
@@ -471,7 +525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3102DB0A-FAFE-4892-A69F-F119129C8B56}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -519,6 +573,168 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E4D8BF-D5B8-4CEF-B366-FC7E28406D6A}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DE6CBDE-DB40-44A8-82DC-20A32EB102D7}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AFDBA09-C936-41B1-8FBF-B5F31D15E41D}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -752,7 +968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B908A32-A6DC-43B6-91F8-CFE179A117E7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -800,4 +1016,182 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AEBEDCA-9E8C-4A29-9DEC-2E85C86A4FCC}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83266BC-7DC0-4A24-902D-283FA7E32344}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FEE2DB-FD93-47A3-ACE1-5FAE1A2F2F04}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>